<commit_message>
Actualización general: cambios en doc y nuevos archivos en output
</commit_message>
<xml_diff>
--- a/output/tiles_por_clase.xlsx
+++ b/output/tiles_por_clase.xlsx
@@ -5,23 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inteia\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inteia\CLC_N3_IA_DianaMillan\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02FA591-055A-40C3-B020-7B073962E130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66424AED-36A9-417A-8B3A-1C347636766A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4416" yWindow="-12960" windowWidth="9432" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10944" yWindow="-12960" windowWidth="15552" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$F$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$A$1:$F$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="51">
   <si>
     <t>tile_id</t>
   </si>
@@ -190,6 +192,9 @@
   </si>
   <si>
     <t>Total general</t>
+  </si>
+  <si>
+    <t>(en blanco)</t>
   </si>
 </sst>
 </file>
@@ -311,6 +316,62 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="diana" refreshedDate="45771.736471643519" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="60" xr:uid="{07E96E15-6652-4345-8D45-07F18BE357E5}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:F1048576" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="tile_id" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="3" maxValue="99"/>
+    </cacheField>
+    <cacheField name="nivel_3" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="AREA_HECTAREAS" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.13449646585402311" maxValue="137.17147140633821"/>
+    </cacheField>
+    <cacheField name="AREA_TOTAL" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="142.48702220528079" maxValue="142.51446841739849"/>
+    </cacheField>
+    <cacheField name="PCT_AREA" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="9.4382963657528953E-4" maxValue="900"/>
+    </cacheField>
+    <cacheField name="leyenda" numFmtId="0">
+      <sharedItems containsBlank="1" count="22">
+        <s v="Tejido urbano discontinuo"/>
+        <s v="Tejido urbano continuo"/>
+        <s v="Zonas verdes urbanas"/>
+        <s v="Instalaciones recreativas"/>
+        <s v="Mosaico de pastos con espacios naturales"/>
+        <s v="Zonas industriales o comerciales"/>
+        <s v="Cultivos permanentes arbustivos"/>
+        <s v="Vegetación secundaria"/>
+        <s v="Mosaico de cultivos, pastos y espacios naturales"/>
+        <s v="Tierras desnudas y degradadas"/>
+        <s v="Zonas de extracción minera"/>
+        <s v="Mosaico de pastos y cultivos"/>
+        <s v="Pastos limpios"/>
+        <s v="Aeropuertos"/>
+        <s v="Mosaico de cultivos y espacios naturales"/>
+        <s v="Plantación forestal"/>
+        <s v="Pastos enmalezados"/>
+        <s v="Ríos (50 m)"/>
+        <s v="Bosque de galería y ripario"/>
+        <s v="Bosque denso"/>
+        <s v="Bosque fragmentado"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="51">
   <r>
@@ -465,12 +526,497 @@
   </r>
   <r>
     <x v="20"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="60">
+  <r>
+    <n v="3"/>
+    <s v="112"/>
+    <n v="44.06418216303171"/>
+    <n v="142.49387972077301"/>
+    <n v="0.30923561243036291"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <s v="111"/>
+    <n v="124.25219001099801"/>
+    <n v="142.49389160779151"/>
+    <n v="0.87198257138626667"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <s v="141"/>
+    <n v="47.879905008019669"/>
+    <n v="142.49387972077301"/>
+    <n v="0.33601376495498469"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <s v="142"/>
+    <n v="9.1449867634417643"/>
+    <n v="142.4938797200256"/>
+    <n v="6.4178102115052177E-2"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <s v="141"/>
+    <n v="14.044715816891291"/>
+    <n v="142.4938797200256"/>
+    <n v="9.8563642484060285E-2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <s v="244"/>
+    <n v="34.414713790378237"/>
+    <n v="142.49389160853991"/>
+    <n v="0.24151711629100961"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <s v="121"/>
+    <n v="23.635666963138039"/>
+    <n v="142.49389160853991"/>
+    <n v="0.1658714397952587"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <s v="222"/>
+    <n v="40.038008803413753"/>
+    <n v="142.4961870062541"/>
+    <n v="0.28097600114490429"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <s v="323"/>
+    <n v="38.033607203242951"/>
+    <n v="142.49617511754479"/>
+    <n v="0.26690967088673861"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <s v="243"/>
+    <n v="41.140794243365129"/>
+    <n v="142.496175118298"/>
+    <n v="0.28871507750443631"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <s v="323"/>
+    <n v="37.067473355686772"/>
+    <n v="142.496175118298"/>
+    <n v="0.26012960225012333"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <s v="121"/>
+    <n v="34.844180564491083"/>
+    <n v="142.49618700549689"/>
+    <n v="0.24452710838604369"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <s v="323"/>
+    <n v="74.103521971195107"/>
+    <n v="142.49617511754329"/>
+    <n v="0.5200386740912033"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <s v="112"/>
+    <n v="30.265144740701839"/>
+    <n v="142.4961870062522"/>
+    <n v="0.21239266380772651"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <s v="222"/>
+    <n v="120.3420463180213"/>
+    <n v="142.49848937914851"/>
+    <n v="0.84451454076698973"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="23"/>
+    <s v="333"/>
+    <n v="16.56262169867211"/>
+    <n v="142.49848937989631"/>
+    <n v="0.11623015633882761"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <s v="333"/>
+    <n v="8.0735442906183543"/>
+    <n v="142.49850126729581"/>
+    <n v="5.6657047048334679E-2"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <s v="131"/>
+    <n v="0.39539842739514458"/>
+    <n v="142.49848937989489"/>
+    <n v="2.774755221025741E-3"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <s v="242"/>
+    <n v="42.628299567968043"/>
+    <n v="142.49850126729771"/>
+    <n v="0.29914910815803031"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <s v="131"/>
+    <n v="14.6926264955551"/>
+    <n v="142.49850126729771"/>
+    <n v="0.103107235268354"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <s v="111"/>
+    <n v="26.276850742502361"/>
+    <n v="142.49850126805279"/>
+    <n v="0.18440089200007229"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <s v="243"/>
+    <n v="137.17147140633821"/>
+    <n v="142.50077494998621"/>
+    <n v="0.96260158202284596"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <n v="33"/>
+    <s v="112"/>
+    <n v="24.928519736047662"/>
+    <n v="142.5007749507389"/>
+    <n v="0.1749360292578423"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="34"/>
+    <s v="231"/>
+    <n v="37.640608999996623"/>
+    <n v="142.50078683833689"/>
+    <n v="0.2641431660493132"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <n v="36"/>
+    <s v="244"/>
+    <n v="110.1666759449614"/>
+    <n v="142.50078683833121"/>
+    <n v="0.77309521153694949"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <s v="124"/>
+    <n v="0.13449646585402311"/>
+    <n v="142.50078683908151"/>
+    <n v="9.4382963657528953E-4"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <s v="111"/>
+    <n v="22.643264789675332"/>
+    <n v="142.50078683908151"/>
+    <n v="0.1588992263968701"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="44"/>
+    <s v="245"/>
+    <n v="41.661660979813298"/>
+    <n v="142.50307938520129"/>
+    <n v="0.29235621545550827"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <n v="48"/>
+    <s v="315"/>
+    <n v="113.9353985730006"/>
+    <n v="142.50306749666521"/>
+    <n v="0.79952944574801432"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="49"/>
+    <s v="233"/>
+    <n v="29.620894502422288"/>
+    <n v="142.5030793859556"/>
+    <n v="0.20786143450414149"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <n v="51"/>
+    <s v="242"/>
+    <n v="96.358706396437398"/>
+    <n v="142.50537890750911"/>
+    <n v="0.6761759249731728"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <n v="53"/>
+    <s v="242"/>
+    <n v="42.728611442539872"/>
+    <n v="142.50536701878869"/>
+    <n v="0.29983861195140998"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <n v="57"/>
+    <s v="315"/>
+    <n v="40.999319126530501"/>
+    <n v="142.50536701878781"/>
+    <n v="0.28770368431895738"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="62"/>
+    <s v="511"/>
+    <n v="13.554849907347529"/>
+    <n v="142.50763784945951"/>
+    <n v="9.5116655583516424E-2"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <n v="66"/>
+    <s v="314"/>
+    <n v="40.513648144703943"/>
+    <n v="142.50764973837579"/>
+    <n v="0.28429104135168443"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <n v="70"/>
+    <s v="222"/>
+    <n v="39.589182792528582"/>
+    <n v="142.48702220528079"/>
+    <n v="0.27784413050258372"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="70"/>
+    <s v="245"/>
+    <n v="35.934810830591601"/>
+    <n v="142.48702220528079"/>
+    <n v="0.25219707924571821"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <n v="71"/>
+    <s v="245"/>
+    <n v="109.1551170324784"/>
+    <n v="142.50993943454171"/>
+    <n v="0.76594739612962903"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <n v="73"/>
+    <s v="511"/>
+    <n v="10.943897216901471"/>
+    <n v="142.5099275454314"/>
+    <n v="7.6793928713581164E-2"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <n v="75"/>
+    <s v="315"/>
+    <n v="33.737955580276733"/>
+    <n v="142.5099275454312"/>
+    <n v="0.23674108998140711"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="77"/>
+    <s v="231"/>
+    <n v="102.87681965995981"/>
+    <n v="142.50992754543049"/>
+    <n v="0.72189230204445831"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <n v="81"/>
+    <s v="231"/>
+    <n v="37.086559361828961"/>
+    <n v="142.51220043874491"/>
+    <n v="0.26023427641740488"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <n v="89"/>
+    <s v="311"/>
+    <n v="24.666548253956559"/>
+    <n v="142.51220043875091"/>
+    <n v="0.17308376530581879"/>
+    <x v="19"/>
+  </r>
+  <r>
+    <n v="94"/>
+    <s v="314"/>
+    <n v="57.891470175027671"/>
+    <n v="142.51446841665771"/>
+    <n v="0.40621468695918789"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <n v="94"/>
+    <s v="243"/>
+    <n v="39.047066328253521"/>
+    <n v="142.51446841665771"/>
+    <n v="0.27398668192828579"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <n v="97"/>
+    <s v="314"/>
+    <n v="42.052375336006378"/>
+    <n v="142.51445652792029"/>
+    <n v="0.29507445322059539"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <n v="98"/>
+    <s v="311"/>
+    <n v="11.0255487815639"/>
+    <n v="142.51445652716711"/>
+    <n v="7.736442358366738E-2"/>
+    <x v="19"/>
+  </r>
+  <r>
+    <n v="98"/>
+    <s v="244"/>
+    <n v="36.822800052340817"/>
+    <n v="142.51445652716711"/>
+    <n v="0.25837940198944948"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="98"/>
+    <s v="233"/>
+    <n v="30.790685911545971"/>
+    <n v="142.51445652716711"/>
+    <n v="0.21605307041729091"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <n v="99"/>
+    <s v="311"/>
+    <n v="104.2751667698341"/>
+    <n v="142.51446841739849"/>
+    <n v="0.73168126666572175"/>
+    <x v="19"/>
+  </r>
+  <r>
+    <n v="99"/>
+    <s v="313"/>
+    <n v="16.377050923498331"/>
+    <n v="142.51446841739849"/>
+    <n v="0.1149150055104088"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="21"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="21"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="21"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="21"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="21"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="21"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="21"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="900"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="21"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6F30C227-E064-4FC2-A6D4-0884151A6800}" name="TablaDinámica1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6F30C227-E064-4FC2-A6D4-0884151A6800}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
   <location ref="A3:A25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" showAll="0">
@@ -566,6 +1112,132 @@
     </i>
     <i>
       <x v="20"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{368DC6FC-5818-45BF-8418-B2DDA5E442A5}" name="TablaDinámica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
+  <location ref="A3:A26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="23">
+        <item x="13"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="4"/>
+        <item x="11"/>
+        <item x="16"/>
+        <item x="12"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="10"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="21"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="23">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
     </i>
     <i t="grand">
       <x/>
@@ -1003,11 +1675,149 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394111ED-F21A-4DBC-B233-116873290868}">
+  <dimension ref="A3:A26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>